<commit_message>
Added more error checking to "2 Analyte" sheet.
</commit_message>
<xml_diff>
--- a/Documents/Automate Templates/Test Event Calculator.xlsx
+++ b/Documents/Automate Templates/Test Event Calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gasleaksensors1-my.sharepoint.com/personal/ajohnson_gasleaksensors_com/Documents/Test Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajohnson\source\repos\Sensit Test Suite\Documents\Automate Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="239" documentId="13_ncr:1_{8099836A-2624-4B11-B609-2936A39A4DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD47E545-DB5C-4FB6-847A-01F6AEDE63E5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A16A75-BF5A-483A-AE35-BECA58CDD871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-45" windowWidth="29040" windowHeight="15645" activeTab="1" xr2:uid="{E7D9A682-83FE-4E0E-B163-912CBE56D6E7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E7D9A682-83FE-4E0E-B163-912CBE56D6E7}"/>
   </bookViews>
   <sheets>
     <sheet name="1 Analyte" sheetId="3" r:id="rId1"/>
@@ -27,17 +27,26 @@
     <definedName name="MFC2Concentration">'2 Analyte'!$E$7</definedName>
     <definedName name="MFC2Ratio" localSheetId="1">'2 Analyte'!$F$7</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>% Analyte</t>
   </si>
@@ -114,12 +123,6 @@
     <t>% H2</t>
   </si>
   <si>
-    <t>CH4 (%V)</t>
-  </si>
-  <si>
-    <t>H2 (%V)</t>
-  </si>
-  <si>
     <t>%V</t>
   </si>
   <si>
@@ -157,6 +160,27 @@
   </si>
   <si>
     <t>Range (%V)</t>
+  </si>
+  <si>
+    <t>H2 / CH4</t>
+  </si>
+  <si>
+    <t>H2 Bottle</t>
+  </si>
+  <si>
+    <t>CH4 Bottle</t>
+  </si>
+  <si>
+    <t>Range(%V):</t>
+  </si>
+  <si>
+    <t>Line Gas H2:</t>
+  </si>
+  <si>
+    <t>Analyte %</t>
+  </si>
+  <si>
+    <t>Error Checking</t>
   </si>
 </sst>
 </file>
@@ -169,7 +193,7 @@
     <numFmt numFmtId="166" formatCode="0.000%"/>
     <numFmt numFmtId="167" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,8 +252,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,8 +285,13 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -301,15 +345,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -333,7 +394,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="6" fillId="3" borderId="1" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="6" fillId="3" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="6" fillId="3" borderId="3" xfId="4" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="6" fillId="3" borderId="1" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -351,8 +411,6 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="3" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -364,6 +422,13 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="4" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="9" fillId="4" borderId="1" xfId="6" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -381,15 +446,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="8" fillId="3" borderId="5" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Heading 1" xfId="3" builtinId="16"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="6" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="5" builtinId="21"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="36">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color rgb="FF3F3F3F"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border outline="0">
+        <right style="thin">
+          <color rgb="FF3F3F3F"/>
+        </right>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
@@ -480,9 +574,6 @@
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="165" formatCode="0.0%"/>
     </dxf>
     <dxf>
@@ -514,6 +605,46 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -536,10 +667,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DA1FD50D-57AC-4199-8989-CAC1CDEDD257}" name="Table1Analyte" displayName="Table1Analyte" ref="C5:E16" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="4" xr3:uid="{44C91331-4C0B-4F93-821D-CC8BE71D553D}" name="Analyte (%)" dataCellStyle="Percent"/>
-    <tableColumn id="1" xr3:uid="{24F15665-90B9-45A1-AEAB-9E49E091E594}" name="Analyte (sccm)" dataDxfId="29">
+    <tableColumn id="1" xr3:uid="{24F15665-90B9-45A1-AEAB-9E49E091E594}" name="Analyte (sccm)" dataDxfId="35">
       <calculatedColumnFormula>Table1Analyte[[#This Row],[Analyte (%)]]*MassFlow</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5A16EE01-2AE8-4AC7-A9FC-4D83104C8283}" name="Diluent (sccm)" dataDxfId="28">
+    <tableColumn id="2" xr3:uid="{5A16EE01-2AE8-4AC7-A9FC-4D83104C8283}" name="Diluent (sccm)" dataDxfId="34">
       <calculatedColumnFormula>MassFlow-Table1Analyte[[#This Row],[Analyte (sccm)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -548,29 +679,35 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1BF40C10-01F5-41BB-857F-F3E02E1EC89F}" name="Table2Analyte" displayName="Table2Analyte" ref="A8:H19" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <tableColumns count="8">
-    <tableColumn id="7" xr3:uid="{0C425943-EB0C-42F2-BE7F-6BCFB4A81178}" name="% Analyte" dataDxfId="25" dataCellStyle="Percent"/>
-    <tableColumn id="10" xr3:uid="{5B413E64-AF06-4A64-899F-08CD2F477F27}" name="% Bottle" dataDxfId="24" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1BF40C10-01F5-41BB-857F-F3E02E1EC89F}" name="Table2Analyte" displayName="Table2Analyte" ref="A8:J19" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <tableColumns count="10">
+    <tableColumn id="7" xr3:uid="{0C425943-EB0C-42F2-BE7F-6BCFB4A81178}" name="% Analyte" dataDxfId="27" dataCellStyle="Percent"/>
+    <tableColumn id="10" xr3:uid="{5B413E64-AF06-4A64-899F-08CD2F477F27}" name="% Bottle" dataDxfId="26" dataCellStyle="Percent">
       <calculatedColumnFormula>Table2Analyte[[#This Row],[% Analyte]] / (MFC1Concentration*MFC1Ratio + MFC2Concentration*MFC2Ratio)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{0EF9062E-AFB5-4AFC-868C-3F684909348E}" name="MFC1 (%)" dataDxfId="23" dataCellStyle="Percent">
+    <tableColumn id="1" xr3:uid="{0EF9062E-AFB5-4AFC-868C-3F684909348E}" name="MFC1 (%)" dataDxfId="25" dataCellStyle="Percent">
       <calculatedColumnFormula>Table2Analyte[[#This Row],[% Bottle]] * MFC1Ratio</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{2D30C2FC-6DA9-4275-90F1-DEC28A67CF85}" name="MFC1 (sccm)" dataDxfId="22">
+    <tableColumn id="5" xr3:uid="{2D30C2FC-6DA9-4275-90F1-DEC28A67CF85}" name="MFC1 (sccm)" dataDxfId="24">
       <calculatedColumnFormula>Table2Analyte[[#This Row],[MFC1 (%)]]*MassFlow</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{3725C7C3-3335-436E-8B30-62C2A6D232D2}" name="MFC2 (%)" dataDxfId="21" dataCellStyle="Percent">
+    <tableColumn id="8" xr3:uid="{3725C7C3-3335-436E-8B30-62C2A6D232D2}" name="MFC2 (%)" dataDxfId="23" dataCellStyle="Percent">
       <calculatedColumnFormula>Table2Analyte[[#This Row],[% Bottle]] * MFC2Ratio</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{14E57EE7-C215-4019-97E6-5A2ABEA60083}" name="MFC2 (sccm)" dataDxfId="20">
+    <tableColumn id="6" xr3:uid="{14E57EE7-C215-4019-97E6-5A2ABEA60083}" name="MFC2 (sccm)" dataDxfId="22">
       <calculatedColumnFormula>Table2Analyte[[#This Row],[MFC2 (%)]]*MassFlow</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{437CC065-AA5D-46CA-93EE-C2CF705D8260}" name="MFC3 (%)" dataDxfId="19" dataCellStyle="Normal">
+    <tableColumn id="2" xr3:uid="{437CC065-AA5D-46CA-93EE-C2CF705D8260}" name="MFC3 (%)" dataDxfId="21" dataCellStyle="Normal">
       <calculatedColumnFormula>100%-Table2Analyte[[#This Row],[MFC1 (%)]]-Table2Analyte[[#This Row],[MFC2 (%)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E1B81695-A4B7-48F4-94B8-836981B0ACE3}" name="MFC3 (sccm)" dataDxfId="18" dataCellStyle="Normal">
+    <tableColumn id="9" xr3:uid="{E1B81695-A4B7-48F4-94B8-836981B0ACE3}" name="MFC3 (sccm)" dataDxfId="2" dataCellStyle="Normal">
       <calculatedColumnFormula>Table2Analyte[[#This Row],[MFC3 (%)]]*MassFlow</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{B6EE30F0-D5BA-4660-BF9C-60E7D343000E}" name="H2 / CH4" dataDxfId="1" dataCellStyle="Output">
+      <calculatedColumnFormula>IF(Table2Analyte[[#This Row],[MFC1 (%)]]+Table2Analyte[[#This Row],[MFC2 (%)]]&lt;&gt;0,Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration / (Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration+Table2Analyte[[#This Row],[MFC1 (%)]]*MFC1Concentration), " - ")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{2397360A-9356-4EC0-836F-7471FA93FA95}" name="Analyte %" dataDxfId="0" dataCellStyle="Percent">
+      <calculatedColumnFormula>(Table2Analyte[[#This Row],[MFC1 (sccm)]]*MFC1Concentration+Table2Analyte[[#This Row],[MFC2 (sccm)]]*MFC2Concentration)/MassFlow</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -578,17 +715,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0E9F21CF-7859-4304-83C4-2967DE9EA1BA}" name="Table15" displayName="Table15" ref="A1:F15" totalsRowShown="0" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0E9F21CF-7859-4304-83C4-2967DE9EA1BA}" name="Table15" displayName="Table15" ref="A1:F16" totalsRowShown="0" dataDxfId="20">
   <tableColumns count="6">
-    <tableColumn id="2" xr3:uid="{F9161B4C-0952-4809-8ED7-2C1CA728623D}" name="CH4 (%V)" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{FAED2144-4FB3-49CB-80AD-4374FF0B8D92}" name="CH4 %Analyte" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{D7C30980-0C97-450B-BD21-AEA7CF381DB7}" name="H2 (%V)" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{344B97C4-B036-4D74-ACBC-01E858D7A8D8}" name="H2 %Analyte" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{03F9B13F-6C7C-4AD7-A2D7-7CCB0ECC42C7}" name="% H2" dataDxfId="12" dataCellStyle="Calculation">
-      <calculatedColumnFormula>(Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]]) / (Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]] + Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{F9161B4C-0952-4809-8ED7-2C1CA728623D}" name="CH4 Bottle" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{FAED2144-4FB3-49CB-80AD-4374FF0B8D92}" name="CH4 %Analyte" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{D7C30980-0C97-450B-BD21-AEA7CF381DB7}" name="H2 Bottle" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{344B97C4-B036-4D74-ACBC-01E858D7A8D8}" name="H2 %Analyte" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{03F9B13F-6C7C-4AD7-A2D7-7CCB0ECC42C7}" name="% H2" dataDxfId="15" dataCellStyle="Calculation">
+      <calculatedColumnFormula>Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]] / (Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]] +Table15[[#This Row],[H2 Bottle]]* Table15[[#This Row],[H2 %Analyte]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{17E10DD9-0B26-4883-8398-1D23A30F97C7}" name="Range (%V)" dataDxfId="11" dataCellStyle="Calculation">
-      <calculatedColumnFormula>(Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{17E10DD9-0B26-4883-8398-1D23A30F97C7}" name="Range (%V)" dataDxfId="14" dataCellStyle="Calculation">
+      <calculatedColumnFormula>(Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -596,24 +733,24 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{46D7189E-652D-47CA-B306-0A5E544049AD}" name="Table1" displayName="Table1" ref="A5:K33" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{46D7189E-652D-47CA-B306-0A5E544049AD}" name="Table1" displayName="Table1" ref="A5:K33" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A5:K33" xr:uid="{80A5895D-A487-4A6C-812C-E5CD17B68514}"/>
   <tableColumns count="11">
-    <tableColumn id="10" xr3:uid="{2C33A0AE-0677-48E2-BAAF-C91DF8250FBE}" name="Desired Analyte" dataDxfId="8" dataCellStyle="Input"/>
-    <tableColumn id="11" xr3:uid="{C6A74467-75FE-4B85-965B-09FCA34CB4D0}" name="Desired O2" dataDxfId="7" dataCellStyle="Input"/>
-    <tableColumn id="1" xr3:uid="{0CDAF8FA-DBD1-4851-914E-2DBC182D23DF}" name="MFC1 (%)" dataDxfId="6" dataCellStyle="Percent"/>
-    <tableColumn id="5" xr3:uid="{F51E41ED-FB65-45D1-99B0-CE0A8A52D037}" name="MFC1 (sccm)" dataDxfId="5">
+    <tableColumn id="10" xr3:uid="{2C33A0AE-0677-48E2-BAAF-C91DF8250FBE}" name="Desired Analyte" dataDxfId="11" dataCellStyle="Input"/>
+    <tableColumn id="11" xr3:uid="{C6A74467-75FE-4B85-965B-09FCA34CB4D0}" name="Desired O2" dataDxfId="10" dataCellStyle="Input"/>
+    <tableColumn id="1" xr3:uid="{0CDAF8FA-DBD1-4851-914E-2DBC182D23DF}" name="MFC1 (%)" dataDxfId="9" dataCellStyle="Percent"/>
+    <tableColumn id="5" xr3:uid="{F51E41ED-FB65-45D1-99B0-CE0A8A52D037}" name="MFC1 (sccm)" dataDxfId="8">
       <calculatedColumnFormula>IF(Table1[[#This Row],[MFC1 (%)]] &lt;&gt; 0, Table1[[#This Row],[MFC1 (%)]]*MassFlow, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2EF83AF1-7F2F-49D3-BA8B-A0EBFE03622A}" name="MFC2 (%)" dataDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{DF70380C-E8D8-4F14-90B5-EBBBC7D59F13}" name="MFC2 (sccm)" dataDxfId="3">
+    <tableColumn id="8" xr3:uid="{2EF83AF1-7F2F-49D3-BA8B-A0EBFE03622A}" name="MFC2 (%)" dataDxfId="7" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{DF70380C-E8D8-4F14-90B5-EBBBC7D59F13}" name="MFC2 (sccm)" dataDxfId="6">
       <calculatedColumnFormula>IF(Table1[[#This Row],[MFC2 (%)]] &lt;&gt; 0, Table1[[#This Row],[MFC2 (%)]]*MassFlow, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{997815A5-57B6-4406-A351-95FBE6B6C9F9}" name="MFC3 (%)" dataDxfId="2" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{D9E47F31-8AC0-41C3-9191-BA216292516A}" name="MFC3 (sccm)" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{997815A5-57B6-4406-A351-95FBE6B6C9F9}" name="MFC3 (%)" dataDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{D9E47F31-8AC0-41C3-9191-BA216292516A}" name="MFC3 (sccm)" dataDxfId="4">
       <calculatedColumnFormula>IF(Table1[[#This Row],[MFC3 (%)]] &lt;&gt; 0, Table1[[#This Row],[MFC3 (%)]]*MassFlow, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{2070FFF8-C610-4645-AA9C-C995FE56D480}" name="MFC4 (%)" dataDxfId="0" dataCellStyle="Normal">
+    <tableColumn id="2" xr3:uid="{2070FFF8-C610-4645-AA9C-C995FE56D480}" name="MFC4 (%)" dataDxfId="3" dataCellStyle="Normal">
       <calculatedColumnFormula>100%-Table1[[#This Row],[MFC1 (%)]]-Table1[[#This Row],[MFC2 (%)]]-Table1[[#This Row],[MFC3 (%)]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{DAC4107B-EAD3-46BB-82AB-335352FA7C75}" name="MFC4 (sccm)" dataCellStyle="Normal">
@@ -939,24 +1076,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="26"/>
+      <c r="A1" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="25"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="24">
+        <v>26</v>
+      </c>
+      <c r="D3" s="23">
         <v>300</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -971,17 +1108,17 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C6" s="25">
+      <c r="C6" s="24">
         <v>0</v>
       </c>
       <c r="D6">
@@ -994,7 +1131,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="25">
+      <c r="C7" s="24">
         <v>0.1</v>
       </c>
       <c r="D7">
@@ -1007,7 +1144,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="25">
+      <c r="C8" s="24">
         <v>0.2</v>
       </c>
       <c r="D8">
@@ -1020,7 +1157,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="25">
+      <c r="C9" s="24">
         <v>0.3</v>
       </c>
       <c r="D9">
@@ -1033,7 +1170,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="25">
+      <c r="C10" s="24">
         <v>0.4</v>
       </c>
       <c r="D10">
@@ -1046,7 +1183,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="25">
+      <c r="C11" s="24">
         <v>0.5</v>
       </c>
       <c r="D11">
@@ -1059,7 +1196,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="25">
+      <c r="C12" s="24">
         <v>0.6</v>
       </c>
       <c r="D12">
@@ -1072,7 +1209,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="25">
+      <c r="C13" s="24">
         <v>0.7</v>
       </c>
       <c r="D13">
@@ -1085,7 +1222,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="25">
+      <c r="C14" s="24">
         <v>0.8</v>
       </c>
       <c r="D14">
@@ -1098,7 +1235,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="25">
+      <c r="C15" s="24">
         <v>0.9</v>
       </c>
       <c r="D15">
@@ -1111,7 +1248,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="25">
+      <c r="C16" s="24">
         <v>1</v>
       </c>
       <c r="D16">
@@ -1137,10 +1274,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{121C708E-7C19-457C-8A85-878B42B0C4F4}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,110 +1292,135 @@
     <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="23">
+        <v>300</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="48">
+        <f>MFC2Concentration*MFC2Ratio/(MFC1Concentration*MFC1Ratio+MFC2Concentration*MFC2Ratio)</f>
+        <v>4.9180327868852458E-2</v>
+      </c>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="36">
+        <f>MFC1Concentration*MFC1Ratio+MFC2Concentration*MFC2Ratio</f>
+        <v>3.0499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="C5" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="44"/>
+      <c r="G5" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="43"/>
+    </row>
+    <row r="6" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="C6" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="D7" s="32">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E7" s="31">
+        <v>0.03</v>
+      </c>
+      <c r="F7" s="32">
+        <v>0.05</v>
+      </c>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="46"/>
+    </row>
+    <row r="8" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="24">
-        <v>300</v>
-      </c>
-      <c r="C3" s="20"/>
-    </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="C5" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="42"/>
-      <c r="G5" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="41"/>
-    </row>
-    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="C6" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="28" t="s">
+      <c r="J8" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="31">
         <v>0</v>
       </c>
-      <c r="E6" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="34">
-        <v>0.1</v>
-      </c>
-      <c r="D7" s="35">
-        <v>0.23749999999999999</v>
-      </c>
-      <c r="E7" s="34">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F7" s="35">
-        <v>0.25</v>
-      </c>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-    </row>
-    <row r="8" spans="1:8" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="36" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="34">
-        <v>0</v>
-      </c>
-      <c r="B9" s="33">
+      <c r="B9" s="30">
         <f>Table2Analyte[[#This Row],[% Analyte]] / (MFC1Concentration*MFC1Ratio + MFC2Concentration*MFC2Ratio)</f>
         <v>0</v>
       </c>
@@ -1286,380 +1448,488 @@
         <f>Table2Analyte[[#This Row],[MFC3 (%)]]*MassFlow</f>
         <v>300</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="34">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="B10" s="33">
+      <c r="I9" s="47" t="str">
+        <f>IF(Table2Analyte[[#This Row],[MFC1 (%)]]+Table2Analyte[[#This Row],[MFC2 (%)]]&lt;&gt;0,Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration / (Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration+Table2Analyte[[#This Row],[MFC1 (%)]]*MFC1Concentration), " - ")</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J9" s="49">
+        <f>(Table2Analyte[[#This Row],[MFC1 (sccm)]]*MFC1Concentration+Table2Analyte[[#This Row],[MFC2 (sccm)]]*MFC2Concentration)/MassFlow</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="31">
+        <v>0.01</v>
+      </c>
+      <c r="B10" s="30">
         <f>Table2Analyte[[#This Row],[% Analyte]] / (MFC1Concentration*MFC1Ratio + MFC2Concentration*MFC2Ratio)</f>
-        <v>9.9999999999999992E-2</v>
+        <v>0.32786885245901642</v>
       </c>
       <c r="C10" s="11">
         <f>Table2Analyte[[#This Row],[% Bottle]] * MFC1Ratio</f>
-        <v>2.3749999999999997E-2</v>
+        <v>9.5081967213114751E-2</v>
       </c>
       <c r="D10">
         <f>Table2Analyte[[#This Row],[MFC1 (%)]]*MassFlow</f>
-        <v>7.1249999999999991</v>
+        <v>28.524590163934427</v>
       </c>
       <c r="E10" s="11">
         <f>Table2Analyte[[#This Row],[% Bottle]] * MFC2Ratio</f>
-        <v>2.4999999999999998E-2</v>
+        <v>1.6393442622950821E-2</v>
       </c>
       <c r="F10">
         <f>Table2Analyte[[#This Row],[MFC2 (%)]]*MassFlow</f>
-        <v>7.4999999999999991</v>
+        <v>4.918032786885246</v>
       </c>
       <c r="G10" s="10">
         <f>100%-Table2Analyte[[#This Row],[MFC1 (%)]]-Table2Analyte[[#This Row],[MFC2 (%)]]</f>
-        <v>0.95124999999999993</v>
+        <v>0.88852459016393437</v>
       </c>
       <c r="H10">
         <f>Table2Analyte[[#This Row],[MFC3 (%)]]*MassFlow</f>
-        <v>285.375</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="34">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="B11" s="33">
+        <v>266.55737704918033</v>
+      </c>
+      <c r="I10" s="47">
+        <f>IF(Table2Analyte[[#This Row],[MFC1 (%)]]+Table2Analyte[[#This Row],[MFC2 (%)]]&lt;&gt;0,Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration / (Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration+Table2Analyte[[#This Row],[MFC1 (%)]]*MFC1Concentration), " - ")</f>
+        <v>4.9180327868852458E-2</v>
+      </c>
+      <c r="J10" s="49">
+        <f>(Table2Analyte[[#This Row],[MFC1 (sccm)]]*MFC1Concentration+Table2Analyte[[#This Row],[MFC2 (sccm)]]*MFC2Concentration)/MassFlow</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="31">
+        <v>0.02</v>
+      </c>
+      <c r="B11" s="30">
         <f>Table2Analyte[[#This Row],[% Analyte]] / (MFC1Concentration*MFC1Ratio + MFC2Concentration*MFC2Ratio)</f>
-        <v>0.19999999999999998</v>
+        <v>0.65573770491803285</v>
       </c>
       <c r="C11" s="11">
         <f>Table2Analyte[[#This Row],[% Bottle]] * MFC1Ratio</f>
-        <v>4.7499999999999994E-2</v>
+        <v>0.1901639344262295</v>
       </c>
       <c r="D11">
         <f>Table2Analyte[[#This Row],[MFC1 (%)]]*MassFlow</f>
-        <v>14.249999999999998</v>
+        <v>57.049180327868854</v>
       </c>
       <c r="E11" s="11">
         <f>Table2Analyte[[#This Row],[% Bottle]] * MFC2Ratio</f>
-        <v>4.9999999999999996E-2</v>
+        <v>3.2786885245901641E-2</v>
       </c>
       <c r="F11">
         <f>Table2Analyte[[#This Row],[MFC2 (%)]]*MassFlow</f>
-        <v>14.999999999999998</v>
+        <v>9.8360655737704921</v>
       </c>
       <c r="G11" s="10">
         <f>100%-Table2Analyte[[#This Row],[MFC1 (%)]]-Table2Analyte[[#This Row],[MFC2 (%)]]</f>
-        <v>0.90249999999999997</v>
+        <v>0.77704918032786885</v>
       </c>
       <c r="H11">
         <f>Table2Analyte[[#This Row],[MFC3 (%)]]*MassFlow</f>
-        <v>270.75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="34">
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="B12" s="33">
+        <v>233.11475409836066</v>
+      </c>
+      <c r="I11" s="47">
+        <f>IF(Table2Analyte[[#This Row],[MFC1 (%)]]+Table2Analyte[[#This Row],[MFC2 (%)]]&lt;&gt;0,Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration / (Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration+Table2Analyte[[#This Row],[MFC1 (%)]]*MFC1Concentration), " - ")</f>
+        <v>4.9180327868852458E-2</v>
+      </c>
+      <c r="J11" s="49">
+        <f>(Table2Analyte[[#This Row],[MFC1 (sccm)]]*MFC1Concentration+Table2Analyte[[#This Row],[MFC2 (sccm)]]*MFC2Concentration)/MassFlow</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="31">
+        <v>0.03</v>
+      </c>
+      <c r="B12" s="30">
         <f>Table2Analyte[[#This Row],[% Analyte]] / (MFC1Concentration*MFC1Ratio + MFC2Concentration*MFC2Ratio)</f>
-        <v>0.3</v>
+        <v>0.98360655737704916</v>
       </c>
       <c r="C12" s="11">
         <f>Table2Analyte[[#This Row],[% Bottle]] * MFC1Ratio</f>
-        <v>7.1249999999999994E-2</v>
+        <v>0.28524590163934421</v>
       </c>
       <c r="D12">
         <f>Table2Analyte[[#This Row],[MFC1 (%)]]*MassFlow</f>
-        <v>21.374999999999996</v>
+        <v>85.573770491803259</v>
       </c>
       <c r="E12" s="11">
         <f>Table2Analyte[[#This Row],[% Bottle]] * MFC2Ratio</f>
-        <v>7.4999999999999997E-2</v>
+        <v>4.9180327868852458E-2</v>
       </c>
       <c r="F12">
         <f>Table2Analyte[[#This Row],[MFC2 (%)]]*MassFlow</f>
-        <v>22.5</v>
+        <v>14.754098360655737</v>
       </c>
       <c r="G12" s="10">
         <f>100%-Table2Analyte[[#This Row],[MFC1 (%)]]-Table2Analyte[[#This Row],[MFC2 (%)]]</f>
-        <v>0.85375000000000001</v>
+        <v>0.66557377049180322</v>
       </c>
       <c r="H12">
         <f>Table2Analyte[[#This Row],[MFC3 (%)]]*MassFlow</f>
-        <v>256.125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="34">
-        <v>0.01</v>
-      </c>
-      <c r="B13" s="33">
+        <v>199.67213114754097</v>
+      </c>
+      <c r="I12" s="47">
+        <f>IF(Table2Analyte[[#This Row],[MFC1 (%)]]+Table2Analyte[[#This Row],[MFC2 (%)]]&lt;&gt;0,Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration / (Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration+Table2Analyte[[#This Row],[MFC1 (%)]]*MFC1Concentration), " - ")</f>
+        <v>4.9180327868852458E-2</v>
+      </c>
+      <c r="J12" s="49">
+        <f>(Table2Analyte[[#This Row],[MFC1 (sccm)]]*MFC1Concentration+Table2Analyte[[#This Row],[MFC2 (sccm)]]*MFC2Concentration)/MassFlow</f>
+        <v>2.9999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="31">
+        <v>0.04</v>
+      </c>
+      <c r="B13" s="30">
         <f>Table2Analyte[[#This Row],[% Analyte]] / (MFC1Concentration*MFC1Ratio + MFC2Concentration*MFC2Ratio)</f>
-        <v>0.39999999999999997</v>
+        <v>1.3114754098360657</v>
       </c>
       <c r="C13" s="11">
         <f>Table2Analyte[[#This Row],[% Bottle]] * MFC1Ratio</f>
-        <v>9.4999999999999987E-2</v>
+        <v>0.38032786885245901</v>
       </c>
       <c r="D13">
         <f>Table2Analyte[[#This Row],[MFC1 (%)]]*MassFlow</f>
-        <v>28.499999999999996</v>
+        <v>114.09836065573771</v>
       </c>
       <c r="E13" s="11">
         <f>Table2Analyte[[#This Row],[% Bottle]] * MFC2Ratio</f>
-        <v>9.9999999999999992E-2</v>
+        <v>6.5573770491803282E-2</v>
       </c>
       <c r="F13">
         <f>Table2Analyte[[#This Row],[MFC2 (%)]]*MassFlow</f>
-        <v>29.999999999999996</v>
+        <v>19.672131147540984</v>
       </c>
       <c r="G13" s="10">
         <f>100%-Table2Analyte[[#This Row],[MFC1 (%)]]-Table2Analyte[[#This Row],[MFC2 (%)]]</f>
-        <v>0.80500000000000005</v>
+        <v>0.55409836065573781</v>
       </c>
       <c r="H13">
         <f>Table2Analyte[[#This Row],[MFC3 (%)]]*MassFlow</f>
-        <v>241.50000000000003</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="34">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="B14" s="33">
+        <v>166.22950819672135</v>
+      </c>
+      <c r="I13" s="47">
+        <f>IF(Table2Analyte[[#This Row],[MFC1 (%)]]+Table2Analyte[[#This Row],[MFC2 (%)]]&lt;&gt;0,Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration / (Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration+Table2Analyte[[#This Row],[MFC1 (%)]]*MFC1Concentration), " - ")</f>
+        <v>4.9180327868852458E-2</v>
+      </c>
+      <c r="J13" s="49">
+        <f>(Table2Analyte[[#This Row],[MFC1 (sccm)]]*MFC1Concentration+Table2Analyte[[#This Row],[MFC2 (sccm)]]*MFC2Concentration)/MassFlow</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="31">
+        <v>0.05</v>
+      </c>
+      <c r="B14" s="30">
         <f>Table2Analyte[[#This Row],[% Analyte]] / (MFC1Concentration*MFC1Ratio + MFC2Concentration*MFC2Ratio)</f>
-        <v>0.5</v>
+        <v>1.639344262295082</v>
       </c>
       <c r="C14" s="11">
         <f>Table2Analyte[[#This Row],[% Bottle]] * MFC1Ratio</f>
-        <v>0.11874999999999999</v>
+        <v>0.47540983606557374</v>
       </c>
       <c r="D14">
         <f>Table2Analyte[[#This Row],[MFC1 (%)]]*MassFlow</f>
-        <v>35.625</v>
+        <v>142.62295081967213</v>
       </c>
       <c r="E14" s="11">
         <f>Table2Analyte[[#This Row],[% Bottle]] * MFC2Ratio</f>
-        <v>0.125</v>
+        <v>8.1967213114754106E-2</v>
       </c>
       <c r="F14">
         <f>Table2Analyte[[#This Row],[MFC2 (%)]]*MassFlow</f>
-        <v>37.5</v>
+        <v>24.590163934426233</v>
       </c>
       <c r="G14" s="10">
         <f>100%-Table2Analyte[[#This Row],[MFC1 (%)]]-Table2Analyte[[#This Row],[MFC2 (%)]]</f>
-        <v>0.75624999999999998</v>
+        <v>0.44262295081967218</v>
       </c>
       <c r="H14">
         <f>Table2Analyte[[#This Row],[MFC3 (%)]]*MassFlow</f>
-        <v>226.875</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="34">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="B15" s="33">
+        <v>132.78688524590166</v>
+      </c>
+      <c r="I14" s="47">
+        <f>IF(Table2Analyte[[#This Row],[MFC1 (%)]]+Table2Analyte[[#This Row],[MFC2 (%)]]&lt;&gt;0,Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration / (Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration+Table2Analyte[[#This Row],[MFC1 (%)]]*MFC1Concentration), " - ")</f>
+        <v>4.9180327868852465E-2</v>
+      </c>
+      <c r="J14" s="49">
+        <f>(Table2Analyte[[#This Row],[MFC1 (sccm)]]*MFC1Concentration+Table2Analyte[[#This Row],[MFC2 (sccm)]]*MFC2Concentration)/MassFlow</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="31">
+        <v>0.06</v>
+      </c>
+      <c r="B15" s="30">
         <f>Table2Analyte[[#This Row],[% Analyte]] / (MFC1Concentration*MFC1Ratio + MFC2Concentration*MFC2Ratio)</f>
-        <v>0.6</v>
+        <v>1.9672131147540983</v>
       </c>
       <c r="C15" s="11">
         <f>Table2Analyte[[#This Row],[% Bottle]] * MFC1Ratio</f>
-        <v>0.14249999999999999</v>
+        <v>0.57049180327868843</v>
       </c>
       <c r="D15">
         <f>Table2Analyte[[#This Row],[MFC1 (%)]]*MassFlow</f>
-        <v>42.749999999999993</v>
+        <v>171.14754098360652</v>
       </c>
       <c r="E15" s="11">
         <f>Table2Analyte[[#This Row],[% Bottle]] * MFC2Ratio</f>
-        <v>0.15</v>
+        <v>9.8360655737704916E-2</v>
       </c>
       <c r="F15">
         <f>Table2Analyte[[#This Row],[MFC2 (%)]]*MassFlow</f>
-        <v>45</v>
+        <v>29.508196721311474</v>
       </c>
       <c r="G15" s="10">
         <f>100%-Table2Analyte[[#This Row],[MFC1 (%)]]-Table2Analyte[[#This Row],[MFC2 (%)]]</f>
-        <v>0.70750000000000002</v>
+        <v>0.33114754098360666</v>
       </c>
       <c r="H15">
         <f>Table2Analyte[[#This Row],[MFC3 (%)]]*MassFlow</f>
-        <v>212.25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="34">
-        <v>1.7500000000000002E-2</v>
-      </c>
-      <c r="B16" s="33">
+        <v>99.344262295082004</v>
+      </c>
+      <c r="I15" s="47">
+        <f>IF(Table2Analyte[[#This Row],[MFC1 (%)]]+Table2Analyte[[#This Row],[MFC2 (%)]]&lt;&gt;0,Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration / (Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration+Table2Analyte[[#This Row],[MFC1 (%)]]*MFC1Concentration), " - ")</f>
+        <v>4.9180327868852458E-2</v>
+      </c>
+      <c r="J15" s="49">
+        <f>(Table2Analyte[[#This Row],[MFC1 (sccm)]]*MFC1Concentration+Table2Analyte[[#This Row],[MFC2 (sccm)]]*MFC2Concentration)/MassFlow</f>
+        <v>5.9999999999999991E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="31">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B16" s="30">
         <f>Table2Analyte[[#This Row],[% Analyte]] / (MFC1Concentration*MFC1Ratio + MFC2Concentration*MFC2Ratio)</f>
-        <v>0.70000000000000007</v>
+        <v>2.2950819672131151</v>
       </c>
       <c r="C16" s="11">
         <f>Table2Analyte[[#This Row],[% Bottle]] * MFC1Ratio</f>
-        <v>0.16625000000000001</v>
+        <v>0.66557377049180333</v>
       </c>
       <c r="D16">
         <f>Table2Analyte[[#This Row],[MFC1 (%)]]*MassFlow</f>
-        <v>49.875</v>
+        <v>199.67213114754099</v>
       </c>
       <c r="E16" s="11">
         <f>Table2Analyte[[#This Row],[% Bottle]] * MFC2Ratio</f>
-        <v>0.17500000000000002</v>
+        <v>0.11475409836065575</v>
       </c>
       <c r="F16">
         <f>Table2Analyte[[#This Row],[MFC2 (%)]]*MassFlow</f>
-        <v>52.500000000000007</v>
+        <v>34.426229508196727</v>
       </c>
       <c r="G16" s="10">
         <f>100%-Table2Analyte[[#This Row],[MFC1 (%)]]-Table2Analyte[[#This Row],[MFC2 (%)]]</f>
-        <v>0.65874999999999995</v>
+        <v>0.21967213114754092</v>
       </c>
       <c r="H16">
         <f>Table2Analyte[[#This Row],[MFC3 (%)]]*MassFlow</f>
-        <v>197.62499999999997</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="34">
-        <v>0.02</v>
-      </c>
-      <c r="B17" s="33">
+        <v>65.901639344262279</v>
+      </c>
+      <c r="I16" s="47">
+        <f>IF(Table2Analyte[[#This Row],[MFC1 (%)]]+Table2Analyte[[#This Row],[MFC2 (%)]]&lt;&gt;0,Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration / (Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration+Table2Analyte[[#This Row],[MFC1 (%)]]*MFC1Concentration), " - ")</f>
+        <v>4.9180327868852458E-2</v>
+      </c>
+      <c r="J16" s="49">
+        <f>(Table2Analyte[[#This Row],[MFC1 (sccm)]]*MFC1Concentration+Table2Analyte[[#This Row],[MFC2 (sccm)]]*MFC2Concentration)/MassFlow</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="31">
+        <v>0.08</v>
+      </c>
+      <c r="B17" s="30">
         <f>Table2Analyte[[#This Row],[% Analyte]] / (MFC1Concentration*MFC1Ratio + MFC2Concentration*MFC2Ratio)</f>
-        <v>0.79999999999999993</v>
+        <v>2.6229508196721314</v>
       </c>
       <c r="C17" s="11">
         <f>Table2Analyte[[#This Row],[% Bottle]] * MFC1Ratio</f>
-        <v>0.18999999999999997</v>
+        <v>0.76065573770491801</v>
       </c>
       <c r="D17">
         <f>Table2Analyte[[#This Row],[MFC1 (%)]]*MassFlow</f>
-        <v>56.999999999999993</v>
+        <v>228.19672131147541</v>
       </c>
       <c r="E17" s="11">
         <f>Table2Analyte[[#This Row],[% Bottle]] * MFC2Ratio</f>
-        <v>0.19999999999999998</v>
+        <v>0.13114754098360656</v>
       </c>
       <c r="F17">
         <f>Table2Analyte[[#This Row],[MFC2 (%)]]*MassFlow</f>
-        <v>59.999999999999993</v>
+        <v>39.344262295081968</v>
       </c>
       <c r="G17" s="10">
         <f>100%-Table2Analyte[[#This Row],[MFC1 (%)]]-Table2Analyte[[#This Row],[MFC2 (%)]]</f>
-        <v>0.6100000000000001</v>
+        <v>0.10819672131147542</v>
       </c>
       <c r="H17">
         <f>Table2Analyte[[#This Row],[MFC3 (%)]]*MassFlow</f>
-        <v>183.00000000000003</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="34">
-        <v>2.2499999999999999E-2</v>
-      </c>
-      <c r="B18" s="33">
+        <v>32.459016393442624</v>
+      </c>
+      <c r="I17" s="47">
+        <f>IF(Table2Analyte[[#This Row],[MFC1 (%)]]+Table2Analyte[[#This Row],[MFC2 (%)]]&lt;&gt;0,Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration / (Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration+Table2Analyte[[#This Row],[MFC1 (%)]]*MFC1Concentration), " - ")</f>
+        <v>4.9180327868852458E-2</v>
+      </c>
+      <c r="J17" s="49">
+        <f>(Table2Analyte[[#This Row],[MFC1 (sccm)]]*MFC1Concentration+Table2Analyte[[#This Row],[MFC2 (sccm)]]*MFC2Concentration)/MassFlow</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="31">
+        <v>0.09</v>
+      </c>
+      <c r="B18" s="30">
         <f>Table2Analyte[[#This Row],[% Analyte]] / (MFC1Concentration*MFC1Ratio + MFC2Concentration*MFC2Ratio)</f>
-        <v>0.89999999999999991</v>
+        <v>2.9508196721311477</v>
       </c>
       <c r="C18" s="11">
         <f>Table2Analyte[[#This Row],[% Bottle]] * MFC1Ratio</f>
-        <v>0.21374999999999997</v>
+        <v>0.8557377049180328</v>
       </c>
       <c r="D18">
         <f>Table2Analyte[[#This Row],[MFC1 (%)]]*MassFlow</f>
-        <v>64.124999999999986</v>
+        <v>256.72131147540983</v>
       </c>
       <c r="E18" s="11">
         <f>Table2Analyte[[#This Row],[% Bottle]] * MFC2Ratio</f>
-        <v>0.22499999999999998</v>
+        <v>0.1475409836065574</v>
       </c>
       <c r="F18">
         <f>Table2Analyte[[#This Row],[MFC2 (%)]]*MassFlow</f>
-        <v>67.5</v>
+        <v>44.262295081967224</v>
       </c>
       <c r="G18" s="10">
         <f>100%-Table2Analyte[[#This Row],[MFC1 (%)]]-Table2Analyte[[#This Row],[MFC2 (%)]]</f>
-        <v>0.56125000000000003</v>
+        <v>-3.2786885245902064E-3</v>
       </c>
       <c r="H18">
         <f>Table2Analyte[[#This Row],[MFC3 (%)]]*MassFlow</f>
-        <v>168.375</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="34">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="B19" s="33">
+        <v>-0.98360655737706193</v>
+      </c>
+      <c r="I18" s="47">
+        <f>IF(Table2Analyte[[#This Row],[MFC1 (%)]]+Table2Analyte[[#This Row],[MFC2 (%)]]&lt;&gt;0,Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration / (Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration+Table2Analyte[[#This Row],[MFC1 (%)]]*MFC1Concentration), " - ")</f>
+        <v>4.9180327868852458E-2</v>
+      </c>
+      <c r="J18" s="49">
+        <f>(Table2Analyte[[#This Row],[MFC1 (sccm)]]*MFC1Concentration+Table2Analyte[[#This Row],[MFC2 (sccm)]]*MFC2Concentration)/MassFlow</f>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="31">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="B19" s="30">
         <f>Table2Analyte[[#This Row],[% Analyte]] / (MFC1Concentration*MFC1Ratio + MFC2Concentration*MFC2Ratio)</f>
-        <v>1</v>
+        <v>3.180327868852459</v>
       </c>
       <c r="C19" s="11">
         <f>Table2Analyte[[#This Row],[% Bottle]] * MFC1Ratio</f>
-        <v>0.23749999999999999</v>
+        <v>0.92229508196721299</v>
       </c>
       <c r="D19">
         <f>Table2Analyte[[#This Row],[MFC1 (%)]]*MassFlow</f>
-        <v>71.25</v>
+        <v>276.68852459016392</v>
       </c>
       <c r="E19" s="11">
         <f>Table2Analyte[[#This Row],[% Bottle]] * MFC2Ratio</f>
-        <v>0.25</v>
+        <v>0.15901639344262297</v>
       </c>
       <c r="F19">
         <f>Table2Analyte[[#This Row],[MFC2 (%)]]*MassFlow</f>
-        <v>75</v>
+        <v>47.704918032786892</v>
       </c>
       <c r="G19" s="10">
         <f>100%-Table2Analyte[[#This Row],[MFC1 (%)]]-Table2Analyte[[#This Row],[MFC2 (%)]]</f>
-        <v>0.51249999999999996</v>
+        <v>-8.1311475409835965E-2</v>
       </c>
       <c r="H19">
         <f>Table2Analyte[[#This Row],[MFC3 (%)]]*MassFlow</f>
-        <v>153.75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
+        <v>-24.39344262295079</v>
+      </c>
+      <c r="I19" s="47">
+        <f>IF(Table2Analyte[[#This Row],[MFC1 (%)]]+Table2Analyte[[#This Row],[MFC2 (%)]]&lt;&gt;0,Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration / (Table2Analyte[[#This Row],[MFC2 (%)]]*MFC2Concentration+Table2Analyte[[#This Row],[MFC1 (%)]]*MFC1Concentration), " - ")</f>
+        <v>4.9180327868852465E-2</v>
+      </c>
+      <c r="J19" s="49">
+        <f>(Table2Analyte[[#This Row],[MFC1 (sccm)]]*MFC1Concentration+Table2Analyte[[#This Row],[MFC2 (sccm)]]*MFC2Concentration)/MassFlow</f>
+        <v>9.6999999999999989E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="40" t="s">
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A22:G22"/>
     <mergeCell ref="G5:H7"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E5:F5"/>
   </mergeCells>
+  <conditionalFormatting sqref="B9:B19">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:C19 E9:E19 G9:G19">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7 C7 B9:B19" xr:uid="{85325902-1F90-4C0D-A708-826633BC533A}">
       <formula1>0</formula1>
@@ -1676,10 +1946,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5AF7E3F-4DF8-4881-9E0C-F6CF9D352C3B}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1694,22 +1964,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
         <v>24</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1726,40 +1996,40 @@
         <v>0.2</v>
       </c>
       <c r="E2" s="15">
-        <f>(Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]]) / (Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]] + Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</f>
+        <f>Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]] / (Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]] +Table15[[#This Row],[H2 Bottle]]* Table15[[#This Row],[H2 %Analyte]])</f>
         <v>0.2</v>
       </c>
       <c r="F2" s="15">
-        <f>(Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</f>
+        <f>(Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]])</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="29">
+      <c r="A3" s="28">
         <v>0.1</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="28">
         <v>0.48</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="29">
         <v>0.03</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="28">
         <v>0.4</v>
       </c>
       <c r="E3" s="15">
-        <f>(Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]]) / (Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]] + Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</f>
+        <f>Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]] / (Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]] +Table15[[#This Row],[H2 Bottle]]* Table15[[#This Row],[H2 %Analyte]])</f>
         <v>0.2</v>
       </c>
       <c r="F3" s="15">
-        <f>(Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</f>
+        <f>(Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]])</f>
         <v>0.06</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="18"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="5"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
@@ -1778,42 +2048,42 @@
         <v>0.15</v>
       </c>
       <c r="E5" s="15">
-        <f>(Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]]) / (Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]] + Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</f>
+        <f>Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]] / (Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]] +Table15[[#This Row],[H2 Bottle]]* Table15[[#This Row],[H2 %Analyte]])</f>
         <v>0.15</v>
       </c>
       <c r="F5" s="15">
-        <f>(Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</f>
+        <f>(Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]])</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+      <c r="A6" s="28">
         <v>0.1</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="28">
         <v>0.51</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="29">
         <v>0.03</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="28">
         <v>0.3</v>
       </c>
-      <c r="E6" s="32">
-        <f>(Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]]) / (Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]] + Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</f>
+      <c r="E6" s="15">
+        <f>Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]] / (Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]] +Table15[[#This Row],[H2 Bottle]]* Table15[[#This Row],[H2 %Analyte]])</f>
         <v>0.14999999999999997</v>
       </c>
-      <c r="F6" s="19">
-        <f>(Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</f>
+      <c r="F6" s="18">
+        <f>(Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]])</f>
         <v>6.0000000000000005E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="18"/>
+      <c r="C7" s="17"/>
       <c r="D7" s="13"/>
-      <c r="E7" s="16"/>
+      <c r="E7" s="15"/>
       <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1830,134 +2100,156 @@
         <v>0.1</v>
       </c>
       <c r="E8" s="15">
-        <f>(Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]]) / (Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]] + Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</f>
+        <f>Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]] / (Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]] +Table15[[#This Row],[H2 Bottle]]* Table15[[#This Row],[H2 %Analyte]])</f>
         <v>0.1</v>
       </c>
       <c r="F8" s="15">
-        <f>(Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</f>
+        <f>(Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]])</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="20">
+      <c r="A9" s="19">
         <v>0.1</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="19">
         <v>0.22500000000000001</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="19">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="19">
         <v>0.5</v>
       </c>
-      <c r="E9" s="19">
-        <f>(Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]]) / (Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]] + Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</f>
+      <c r="E9" s="15">
+        <f>Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]] / (Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]] +Table15[[#This Row],[H2 Bottle]]* Table15[[#This Row],[H2 %Analyte]])</f>
         <v>9.9999999999999992E-2</v>
       </c>
-      <c r="F9" s="19">
-        <f>(Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</f>
+      <c r="F9" s="18">
+        <f>(Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]])</f>
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+    <row r="10" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="5"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
+      <c r="F10" s="16"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="B11" s="37">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="C11" s="38">
+        <v>0.03</v>
+      </c>
+      <c r="D11" s="37">
+        <v>0.05</v>
+      </c>
+      <c r="E11" s="15">
+        <f>Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]] / (Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]] +Table15[[#This Row],[H2 Bottle]]* Table15[[#This Row],[H2 %Analyte]])</f>
+        <v>0.05</v>
+      </c>
+      <c r="F11" s="39">
+        <f>(Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]])</f>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
         <v>1</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B12" s="5">
         <v>0.95</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C12" s="5">
         <v>1</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D12" s="5">
         <v>0.05</v>
       </c>
-      <c r="E11" s="17">
-        <f>(Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]]) / (Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]] + Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</f>
+      <c r="E12" s="15">
+        <f>Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]] / (Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]] +Table15[[#This Row],[H2 Bottle]]* Table15[[#This Row],[H2 %Analyte]])</f>
         <v>0.05</v>
       </c>
-      <c r="F11" s="15">
-        <f>(Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</f>
+      <c r="F12" s="15">
+        <f>(Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="27">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="26">
         <v>0.1</v>
       </c>
-      <c r="B12" s="27">
+      <c r="B13" s="26">
         <f>47.5%/2</f>
         <v>0.23749999999999999</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C13" s="29">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D13" s="28">
         <v>0.25</v>
       </c>
-      <c r="E12" s="31">
-        <f>(Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]]) / (Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]] + Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</f>
+      <c r="E13" s="15">
+        <f>Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]] / (Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]] +Table15[[#This Row],[H2 Bottle]]* Table15[[#This Row],[H2 %Analyte]])</f>
         <v>4.9999999999999996E-2</v>
       </c>
-      <c r="F12" s="19">
-        <f>(Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</f>
+      <c r="F13" s="18">
+        <f>(Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]])</f>
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-    </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="17"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
         <v>1</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B15" s="5">
         <v>1</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="5">
+      <c r="C15" s="17"/>
+      <c r="D15" s="5">
         <v>0</v>
       </c>
-      <c r="E14" s="17">
-        <f>(Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]]) / (Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]] + Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</f>
+      <c r="E15" s="15">
+        <f>Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]] / (Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]] +Table15[[#This Row],[H2 Bottle]]* Table15[[#This Row],[H2 %Analyte]])</f>
         <v>0</v>
       </c>
-      <c r="F14" s="15">
-        <f>(Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</f>
+      <c r="F15" s="15">
+        <f>(Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="21">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="20">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="B15" s="22">
+      <c r="B16" s="21">
         <v>1</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="13">
+      <c r="C16" s="20"/>
+      <c r="D16" s="13">
         <v>0</v>
       </c>
-      <c r="E15" s="17">
-        <f>(Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]]) / (Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]] + Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</f>
+      <c r="E16" s="15">
+        <f>Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]] / (Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]] +Table15[[#This Row],[H2 Bottle]]* Table15[[#This Row],[H2 %Analyte]])</f>
         <v>0</v>
       </c>
-      <c r="F15" s="23">
-        <f>(Table15[[#This Row],[CH4 (%V)]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 (%V)]]*Table15[[#This Row],[H2 %Analyte]])</f>
+      <c r="F16" s="22">
+        <f>(Table15[[#This Row],[CH4 Bottle]]*Table15[[#This Row],[CH4 %Analyte]]+Table15[[#This Row],[H2 Bottle]]*Table15[[#This Row],[H2 %Analyte]])</f>
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -1974,7 +2266,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2001,65 +2293,65 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44" t="s">
+      <c r="D2" s="46"/>
+      <c r="E2" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44" t="s">
+      <c r="F2" s="46"/>
+      <c r="G2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44" t="s">
+      <c r="H2" s="46"/>
+      <c r="I2" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="44"/>
+      <c r="J2" s="46"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="43">
+      <c r="C3" s="45">
         <v>1</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43">
+      <c r="D3" s="45"/>
+      <c r="E3" s="45">
         <v>0.04</v>
       </c>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43">
+      <c r="F3" s="45"/>
+      <c r="G3" s="45">
         <v>0</v>
       </c>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43">
+      <c r="H3" s="45"/>
+      <c r="I3" s="45">
         <v>0</v>
       </c>
-      <c r="J3" s="43"/>
+      <c r="J3" s="45"/>
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="43">
+      <c r="C4" s="45">
         <v>0</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43">
+      <c r="D4" s="45"/>
+      <c r="E4" s="45">
         <v>0</v>
       </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43">
+      <c r="F4" s="45"/>
+      <c r="G4" s="45">
         <v>1</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43">
+      <c r="H4" s="45"/>
+      <c r="I4" s="45">
         <v>0.2</v>
       </c>
-      <c r="J4" s="43"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3181,12 +3473,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E0AD433264DC4B4CA4CF2CCA809E77E3" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c23069d77da0a5505d1734b0e66d3f23">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6e9d2e64-bfff-492e-a481-88602d74a0c8" xmlns:ns3="e74f4e40-f96b-4ce9-b9f7-d9180fbf27a9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="450abc95ea8486afe6590bf5e2cc0650" ns2:_="" ns3:_="">
     <xsd:import namespace="6e9d2e64-bfff-492e-a481-88602d74a0c8"/>
@@ -3397,6 +3683,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CD20DC9-775B-4FF8-A400-9D40EAC09B82}">
   <ds:schemaRefs>
@@ -3406,15 +3698,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF5FD629-2682-4C12-BB4D-2EFCB5A65186}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F0A87D6-ADC2-4035-B4B0-FB1911936AD3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3431,4 +3714,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF5FD629-2682-4C12-BB4D-2EFCB5A65186}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>